<commit_message>
Update EMSC stats to include edition 17
</commit_message>
<xml_diff>
--- a/CountryRankingAfterE17.xlsx
+++ b/CountryRankingAfterE17.xlsx
@@ -43052,7 +43052,7 @@
         <v>0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,00,2,0,1,0,1,0,0,0,2,2,0,2,0,1,0,0,0,0,1,0,0,0,1,2,0,0,0,0,0,0,0,0,0,0,0,0,00,3,1,0,0,2,0,1,0,0,0,1,0,0,0,0,1,0,1,1,2,0,1,0,0,0,1,0,1,1,0,0,0,0,0,0,0,00,0,0,1,1,1,2,1,1,1,0,0,0,2,1,0,1,1,1,0,0,0,0,0,1,0,0,1,1,0,0,0,0,0,0,0,0,00,1,0,0,0,0,1,1,2,1,0,1,1,0,2,0,1,2,0,0,0,0,0,0,1,0,1,1,0,0,0,0,0,0,0,0,0,00,0,2,0,0,0,0,1,0,0,3,0,0,0,1,0,1,1,1,0,1,1,0,0,1,0,0,0,0,0,0,0,1,0,0,0,0,00,0,1,1,0,0,0,0,0,0,2,0,0,0,1,1,2,0,1,2,2,0,0,0,0,1,0,0,0,0,0,0,0,0,0,0,0,00,0,1,0,0,0,0,1,0,1,1,1,0,0,0,0,0,0,0,1,0,0,0,0,0,1,0,1,2,1,0,0,0,0,0,0,0,00,0,0,1,0,1,0,1,1,0,0,0,0,2,0,0,0,3,0,1,0,1,0,1,0,1,0,1,0,0,1,0,0,0,0,0,0,00,0,1,0,0,0,0,1,1,0,0,1,1,0,0,0,0,0,1,0,0,1,1,0,0,0,2,1,1,0,0,0,0,0,0,0,0,00,0,0,0,0,0,0,0,0,0,0,0,0,0,0,2,0,0,0,0,0,0,0,0,0,0,0,0,0,1,0,0,0,0,0,0,0,00,0,0,0,0,0,0,0,1,0,0,0,1,0,1,0,0,0,0,0,0,0,0,1,0,0,2,0,1,3,0,0,0,0,0,0,0,0</v>
       </c>
       <c r="V3" s="1" t="str">
-        <v>0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,02,0,2,2,2,1,3,0,1,0,2,0,0,0,0,0,0,0,0,0,0,0,0,03,2,2,2,1,2,0,0,0,1,0,1,0,1,0,1,1,0,0,0,0,0,0,00,2,1,2,4,3,1,0,2,0,0,0,0,0,1,1,0,0,0,0,0,0,0,00,1,1,3,1,1,2,2,0,0,2,0,1,1,1,0,0,0,0,0,0,0,0,00,0,1,1,3,1,2,1,2,0,1,0,1,0,0,0,0,0,0,1,0,0,0,00,0,1,1,0,1,1,4,2,0,2,1,1,0,0,0,0,0,0,0,0,0,0,00,2,1,1,1,0,0,0,0,0,0,2,0,0,1,2,1,0,0,0,0,0,0,00,0,1,2,1,0,2,1,1,0,1,1,3,0,1,0,0,1,0,0,0,0,0,00,0,1,1,1,1,0,0,1,0,1,2,0,2,1,1,0,0,0,0,0,0,0,00,0,0,0,0,0,0,0,0,0,0,1,1,0,0,0,1,0,0,0,0,0,0,00,0,0,0,0,0,1,0,0,0,0,2,1,2,0,1,3,0,0,0,0,0,0,0</v>
+        <v>0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,0,02,0,2,2,2,1,3,0,1,0,2,0,0,0,0,0,0,0,0,0,0,0,0,03,2,2,2,1,2,0,0,0,1,0,1,0,1,0,1,1,0,0,0,0,0,0,00,2,1,2,4,3,1,0,2,0,0,0,0,0,1,1,0,0,0,0,0,0,0,00,1,1,3,1,1,2,2,0,0,2,0,1,1,1,0,0,0,0,0,0,0,0,00,0,1,1,3,1,2,1,2,0,1,0,1,0,0,0,0,0,0,1,0,0,0,00,0,2,0,0,1,1,4,2,0,2,1,1,0,0,0,0,0,0,0,0,0,0,00,2,1,1,1,0,0,0,0,0,0,2,0,0,1,2,1,0,0,0,0,0,0,00,0,1,2,1,0,2,1,1,0,1,1,3,0,1,0,0,1,0,0,0,0,0,00,0,1,1,1,1,0,0,1,0,1,2,0,2,1,1,0,0,0,0,0,0,0,00,0,0,0,0,0,0,0,0,0,0,1,1,0,0,0,1,0,0,0,0,0,0,00,0,0,0,0,0,1,0,0,0,0,2,1,2,0,1,3,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="4">
@@ -52396,52 +52396,52 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="str">
-        <v>Israel</v>
+        <v>The Netherlands</v>
       </c>
       <c r="C24" s="1" t="str">
-        <v>🇮🇱</v>
+        <v>🇳🇱</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J24" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L24" s="1">
         <v>0</v>
       </c>
       <c r="M24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N24" s="1">
         <v>1</v>
       </c>
       <c r="O24" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
       </c>
       <c r="Q24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R24" s="1">
         <v>0</v>
@@ -52450,7 +52450,7 @@
         <v>0</v>
       </c>
       <c r="T24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U24" s="1">
         <v>0</v>
@@ -52476,10 +52476,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="str">
-        <v>Ukraine</v>
+        <v>Israel</v>
       </c>
       <c r="C25" s="1" t="str">
-        <v>🇺🇦</v>
+        <v>🇮🇱</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -52491,31 +52491,31 @@
         <v>2</v>
       </c>
       <c r="G25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L25" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" s="1">
         <v>1</v>
       </c>
       <c r="O25" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P25" s="1">
         <v>0</v>
@@ -52524,13 +52524,13 @@
         <v>1</v>
       </c>
       <c r="R25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U25" s="1">
         <v>0</v>
@@ -52556,10 +52556,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="str">
-        <v>Finland</v>
+        <v>Ukraine</v>
       </c>
       <c r="C26" s="1" t="str">
-        <v>🇫🇮</v>
+        <v>🇺🇦</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -52568,46 +52568,46 @@
         <v>1</v>
       </c>
       <c r="F26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H26" s="1">
         <v>1</v>
       </c>
       <c r="I26" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J26" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K26" s="1">
         <v>2</v>
       </c>
       <c r="L26" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26" s="1">
         <v>0</v>
       </c>
       <c r="Q26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" s="1">
         <v>0</v>
@@ -52616,7 +52616,7 @@
         <v>0</v>
       </c>
       <c r="V26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W26" s="1">
         <v>0</v>
@@ -52636,10 +52636,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="str">
-        <v>Belgium</v>
+        <v>Finland</v>
       </c>
       <c r="C27" s="1" t="str">
-        <v>🇧🇪</v>
+        <v>🇫🇮</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
@@ -52651,19 +52651,19 @@
         <v>1</v>
       </c>
       <c r="G27" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H27" s="1">
         <v>1</v>
       </c>
       <c r="I27" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L27" s="1">
         <v>0</v>
@@ -52672,19 +52672,19 @@
         <v>1</v>
       </c>
       <c r="N27" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P27" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S27" s="1">
         <v>0</v>
@@ -52696,7 +52696,7 @@
         <v>0</v>
       </c>
       <c r="V27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W27" s="1">
         <v>0</v>
@@ -52716,10 +52716,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="str">
-        <v>Austria</v>
+        <v>Belgium</v>
       </c>
       <c r="C28" s="1" t="str">
-        <v>🇦🇹</v>
+        <v>🇧🇪</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -52731,40 +52731,40 @@
         <v>1</v>
       </c>
       <c r="G28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="1">
         <v>1</v>
       </c>
       <c r="I28" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L28" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M28" s="1">
         <v>1</v>
       </c>
       <c r="N28" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O28" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P28" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S28" s="1">
         <v>0</v>
@@ -52796,10 +52796,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="str">
-        <v>The Netherlands</v>
+        <v>Austria</v>
       </c>
       <c r="C29" s="1" t="str">
-        <v>🇳🇱</v>
+        <v>🇦🇹</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
@@ -52817,28 +52817,28 @@
         <v>1</v>
       </c>
       <c r="I29" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J29" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K29" s="1">
         <v>2</v>
       </c>
       <c r="L29" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P29" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q29" s="1">
         <v>0</v>

</xml_diff>